<commit_message>
Adduct mass capabilities added
</commit_message>
<xml_diff>
--- a/inst/extdata/Glycans_Defaults.xlsx
+++ b/inst/extdata/Glycans_Defaults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lewi052/ProteoMatch/IsoMatchMS/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/degn400/Git_Repos/IsoMatchMS/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC63CDC-A2EA-294D-9D59-385C046A29B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0C5237-E917-A944-A7F4-D28276CE8DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{BCF05018-B741-AE44-B44A-5FA14C1D9CFF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Parameter</t>
   </si>
@@ -129,16 +129,19 @@
     <t>AdductLabels</t>
   </si>
   <si>
-    <t>proton</t>
-  </si>
-  <si>
-    <t>Labels for the AdductMasses. Should be separated by a comma with no space (ex. proton,sodium)</t>
-  </si>
-  <si>
     <t>AdductMasses</t>
   </si>
   <si>
-    <t>Masses for the Adducts. Should be separated by a comma with no space (ex. proton,sodium)</t>
+    <t>Labels for the Adduct Masses. Should be separated by a comma with no space (ex. proton,sodium)</t>
+  </si>
+  <si>
+    <t>proton,sodium</t>
+  </si>
+  <si>
+    <t>1.00727647,22.98977</t>
+  </si>
+  <si>
+    <t>Masses for the Adducts. Should be separated by a comma with no space (ex. 1.00727647,22.98977)</t>
   </si>
 </sst>
 </file>
@@ -155,9 +158,9 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Helvetica"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,8 +185,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +504,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,185 +516,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>0.01</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>0.7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>50</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="b">
+      <c r="B9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13">
-        <v>1.0072764700000001</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>34</v>
+      <c r="D13" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing up the main function
</commit_message>
<xml_diff>
--- a/inst/extdata/Glycans_Defaults.xlsx
+++ b/inst/extdata/Glycans_Defaults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/degn400/Git_Repos/IsoMatchMS/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F2988F-F7E1-C243-9089-71707568C218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1746FFD-17EA-A545-A0BD-4D4A45FCE976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{BCF05018-B741-AE44-B44A-5FA14C1D9CFF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Parameter</t>
   </si>
@@ -90,42 +90,18 @@
     <t>The minimum correlation value to consider when generating the trelliscope display</t>
   </si>
   <si>
-    <t>The minimum and maximum number of isotopes to consider</t>
-  </si>
-  <si>
-    <t>IsotopeRange</t>
-  </si>
-  <si>
-    <t>3,20</t>
-  </si>
-  <si>
-    <t>MinimumAbundance</t>
-  </si>
-  <si>
     <t>AddMAI</t>
   </si>
   <si>
-    <t xml:space="preserve">The minimum abundance permitted to be matched. Default is 0.1 which is 0.1%. This is also the minimum change between peaks required for matching. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Add most abundant isotope to the molecular formula calculation step. Warning: This will slow down the tool. </t>
   </si>
   <si>
     <t>Occasionally</t>
   </si>
   <si>
-    <t xml:space="preserve"> 'closest peak' selects the closest peak in the m/z window (recommended for peptides/digested experiments/bottom-up/middle-down) and 'highest abundance' selects the highest abundance peak in the m/z window (recommended for intact protein/top-down)</t>
-  </si>
-  <si>
-    <t>MatchingAlgorithm</t>
-  </si>
-  <si>
     <t>0-6000</t>
   </si>
   <si>
-    <t>closest peak</t>
-  </si>
-  <si>
     <t>AdductLabels</t>
   </si>
   <si>
@@ -142,6 +118,27 @@
   </si>
   <si>
     <t>Masses for the Adducts. Should be separated by a comma with no space (ex. 1.00727647,22.98977)</t>
+  </si>
+  <si>
+    <t>AbundanceThreshold</t>
+  </si>
+  <si>
+    <t>The +/- percent abundance an isotope peak can vary and still be considered a match. If 50%, and the calculated abundance is 3, the matched abundance can vary from 1.5-4</t>
+  </si>
+  <si>
+    <t>IsotopeMinimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The minimum number of isotopes to consider. We recommend 5 for intact proteomics, and 2 or 3 otherwise. </t>
+  </si>
+  <si>
+    <t>IsotopingAlgorithm</t>
+  </si>
+  <si>
+    <t>Rdisop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Either "Rdisop" or "isopat". "Rdisop" is more accurate and recommended, though may crash on windows OS. "isopat" may then be used as an alternative. </t>
   </si>
 </sst>
 </file>
@@ -186,7 +183,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25419109-B18E-184C-810E-4DA843070287}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,7 +531,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -573,129 +570,135 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1">
-        <v>0.01</v>
+        <v>0.7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1">
-        <v>0.7</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="b">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2">
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>6</v>
+      <c r="D11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>35</v>
-      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>